<commit_message>
Both monte carlo and matrix working
</commit_message>
<xml_diff>
--- a/hw3/OpenMP/results.xlsx
+++ b/hw3/OpenMP/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Matrix Add 100x100 Run #1</t>
   </si>
@@ -36,12 +36,6 @@
   </si>
   <si>
     <t>Matrix Add 100x100 Run #4</t>
-  </si>
-  <si>
-    <t>Matrix Add 10000x10000 Run #1</t>
-  </si>
-  <si>
-    <t>Matrix Add 10000x10000 Run #2</t>
   </si>
   <si>
     <t>Pi Run #1</t>
@@ -56,13 +50,16 @@
     <t>Pi Run #4</t>
   </si>
   <si>
-    <t>Matrix Add 10000x10000 Run #3</t>
+    <t>Matrix Add 1000x1000 Run #1</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Matrix Add 1000x1000 Run #2</t>
   </si>
   <si>
-    <t>Matrix Add 10000x10000 Run #4</t>
+    <t>Matrix Add 1000x1000 Run #3</t>
+  </si>
+  <si>
+    <t>Matrix Add 1000x1000 Run #4</t>
   </si>
 </sst>
 </file>
@@ -132,6 +129,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Monti Carlo Multithreading</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -611,11 +633,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="500304496"/>
-        <c:axId val="500305280"/>
+        <c:axId val="190007424"/>
+        <c:axId val="190010168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="500304496"/>
+        <c:axId val="190007424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +680,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500305280"/>
+        <c:crossAx val="190010168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -666,7 +688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="500305280"/>
+        <c:axId val="190010168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,7 +739,655 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500304496"/>
+        <c:crossAx val="190007424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>1000 x 1000 Matrix Multiply</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Matrix Add 1000x1000 Run #1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$19:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$19:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20551</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6937</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6567</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6478</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6783</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6881</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4360</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Matrix Add 1000x1000 Run #2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$19:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$19:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>22126</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12275</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6874</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7293</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6516</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4626</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Matrix Add 1000x1000 Run #3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$19:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$19:$J$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>20801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6739</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6927</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6461</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6531</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4479</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4414</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Matrix Add 1000x1000 Run #4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$G$19:$G$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$19:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>21785</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6968</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6566</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6693</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6607</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4468</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="438076312"/>
+        <c:axId val="438076704"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="438076312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="438076704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="438076704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="438076312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -838,6 +1508,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1354,20 +2064,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>157161</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1905000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1381,6 +2607,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1654,8 +2910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,21 +2949,117 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -1737,22 +3089,118 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>20551</v>
+      </c>
+      <c r="C8">
+        <v>11985</v>
+      </c>
+      <c r="D8">
+        <v>6937</v>
+      </c>
+      <c r="E8">
+        <v>6567</v>
+      </c>
+      <c r="F8">
+        <v>6478</v>
+      </c>
+      <c r="G8">
+        <v>6783</v>
+      </c>
+      <c r="H8">
+        <v>6881</v>
+      </c>
+      <c r="I8">
+        <v>4360</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>22126</v>
+      </c>
+      <c r="C9">
+        <v>12275</v>
+      </c>
+      <c r="D9">
+        <v>6874</v>
+      </c>
+      <c r="E9">
+        <v>7293</v>
+      </c>
+      <c r="F9">
+        <v>6496</v>
+      </c>
+      <c r="G9">
+        <v>6516</v>
+      </c>
+      <c r="H9">
+        <v>4626</v>
+      </c>
+      <c r="I9">
+        <v>4425</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10">
+        <v>20801</v>
+      </c>
+      <c r="C10">
+        <v>12259</v>
+      </c>
+      <c r="D10">
+        <v>6739</v>
+      </c>
+      <c r="E10">
+        <v>6927</v>
+      </c>
+      <c r="F10">
+        <v>6461</v>
+      </c>
+      <c r="G10">
+        <v>6531</v>
+      </c>
+      <c r="H10">
+        <v>4479</v>
+      </c>
+      <c r="I10">
+        <v>4414</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>21785</v>
+      </c>
+      <c r="C11">
+        <v>12609</v>
+      </c>
+      <c r="D11">
+        <v>6968</v>
+      </c>
+      <c r="E11">
+        <v>6566</v>
+      </c>
+      <c r="F11">
+        <v>6693</v>
+      </c>
+      <c r="G11">
+        <v>6607</v>
+      </c>
+      <c r="H11">
+        <v>4468</v>
+      </c>
+      <c r="I11">
+        <v>4375</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1783,7 +3231,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>35514</v>
@@ -1812,7 +3260,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>33614</v>
@@ -1841,7 +3289,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>32754</v>
@@ -1870,7 +3318,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>32804</v>
@@ -1899,16 +3347,28 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" t="s">
+      <c r="H18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" t="s">
+      <c r="I18" t="s">
         <v>9</v>
+      </c>
+      <c r="J18" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1927,6 +3387,21 @@
       <c r="E19">
         <v>32804</v>
       </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>20551</v>
+      </c>
+      <c r="I19">
+        <v>22126</v>
+      </c>
+      <c r="J19">
+        <v>20801</v>
+      </c>
+      <c r="K19">
+        <v>21785</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -1944,8 +3419,20 @@
       <c r="E20">
         <v>20460</v>
       </c>
-      <c r="K20" t="s">
-        <v>11</v>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>11985</v>
+      </c>
+      <c r="I20">
+        <v>12275</v>
+      </c>
+      <c r="J20">
+        <v>12259</v>
+      </c>
+      <c r="K20">
+        <v>12609</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1964,6 +3451,21 @@
       <c r="E21">
         <v>8062</v>
       </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>6937</v>
+      </c>
+      <c r="I21">
+        <v>6874</v>
+      </c>
+      <c r="J21">
+        <v>6739</v>
+      </c>
+      <c r="K21">
+        <v>6968</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1981,6 +3483,21 @@
       <c r="E22">
         <v>6198</v>
       </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>6567</v>
+      </c>
+      <c r="I22">
+        <v>7293</v>
+      </c>
+      <c r="J22">
+        <v>6927</v>
+      </c>
+      <c r="K22">
+        <v>6566</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1998,6 +3515,21 @@
       <c r="E23">
         <v>6214</v>
       </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>6478</v>
+      </c>
+      <c r="I23">
+        <v>6496</v>
+      </c>
+      <c r="J23">
+        <v>6461</v>
+      </c>
+      <c r="K23">
+        <v>6693</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2015,6 +3547,21 @@
       <c r="E24">
         <v>6150</v>
       </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>6783</v>
+      </c>
+      <c r="I24">
+        <v>6516</v>
+      </c>
+      <c r="J24">
+        <v>6531</v>
+      </c>
+      <c r="K24">
+        <v>6607</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -2032,6 +3579,21 @@
       <c r="E25">
         <v>6210</v>
       </c>
+      <c r="G25">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>6881</v>
+      </c>
+      <c r="I25">
+        <v>4626</v>
+      </c>
+      <c r="J25">
+        <v>4479</v>
+      </c>
+      <c r="K25">
+        <v>4468</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -2048,6 +3610,21 @@
       </c>
       <c r="E26">
         <v>6141</v>
+      </c>
+      <c r="G26">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <v>4360</v>
+      </c>
+      <c r="I26">
+        <v>4425</v>
+      </c>
+      <c r="J26">
+        <v>4414</v>
+      </c>
+      <c r="K26">
+        <v>4375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>